<commit_message>
Update spreadsheet with links
</commit_message>
<xml_diff>
--- a/green_storm_components.xlsx
+++ b/green_storm_components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamh/Dev/project_green_storm_zoom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4785FFBE-B395-D94B-AEC7-5C5A763CDADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CC3BF6-3F5C-BB48-8FAF-DEC680C05D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{848B8F3C-E93F-AF40-B020-188FFFBA82D8}"/>
+    <workbookView xWindow="780" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{848B8F3C-E93F-AF40-B020-188FFFBA82D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Ref</t>
   </si>
@@ -235,9 +235,6 @@
     <t>AMS1117-3.3</t>
   </si>
   <si>
-    <t>Rua Dr. Joaquim Eleutério Gaspar Gomes, 24A, 1°</t>
-  </si>
-  <si>
     <t>1A Low Dropout regulator, positive, 3.3V fixed output, SOT-223</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>STM32F103C8Tx</t>
   </si>
   <si>
-    <t>Queluz, Portugal 2745-133</t>
-  </si>
-  <si>
     <t>STMicroelectronics Arm Cortex-M3 MCU, 64KB flash, 20KB RAM, 72 MHz, 2.0-3.6V, 37 GPIO, LQFP48</t>
   </si>
   <si>
@@ -281,16 +275,51 @@
   </si>
   <si>
     <t>Soldered by Hand</t>
+  </si>
+  <si>
+    <t>Weblink</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/KEMET/C0805C226K9PACTU?qs=CmJlwSR1kv6i2XEByn7wWw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/KEMET/C0402C104M8RACTU?qs=JZ1tlzCDhS7uhzdC49Oqsw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/KYOCERA-AVX/04026D100JAT2A?qs=gEbkM7q0lx%252BmQLS7sqmBjQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/Wurth-Elektronik/629105150521?qs=a9WhcLg8qCzXiH7kZP8GRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/Samtec/TSW-104-24-T-S?qs=rU5fayqh%252BE1bToqLrwjy0g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/CK/PCM12SMTBR?qs=By6Nw2ByBD1OEOnWcdZb2g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/ProductDetail/KYOCERA-AVX/CX3225GB16000P0HPQCC?qs=k8ubvZJoN9DNOrO2n3iGnA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.pt/pt/products/detail/laird-signal-integrity-products/LI0603G121R-10/806607?s=N4IgTCBcDa4CwAYC0YDMA2A7CpA5AIiALoC%2BQA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,15 +354,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421B838E-AECC-A54B-BD5D-8E498CCDC5BB}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,10 +692,11 @@
     <col min="4" max="4" width="42.5" customWidth="1"/>
     <col min="6" max="6" width="56.1640625" customWidth="1"/>
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.5" customWidth="1"/>
     <col min="12" max="12" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,8 +721,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -714,8 +750,11 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -735,7 +774,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -760,8 +799,11 @@
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -781,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -801,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -826,8 +868,11 @@
       <c r="H7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -847,7 +892,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -872,8 +917,11 @@
       <c r="H9" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -898,8 +946,11 @@
       <c r="H10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -924,8 +975,11 @@
       <c r="H11" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -945,7 +999,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -968,10 +1022,10 @@
         <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
@@ -996,8 +1050,11 @@
       <c r="H14" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1007,81 +1064,88 @@
       <c r="C15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18">
         <f>SUM(B2:B17)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{4DAF4FF6-3452-F64B-9A59-C8B6E1A145BC}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{4C823E93-B456-D649-9496-D3F4924591B4}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{C8B637D4-E44F-7B4D-B34A-59602949EE5C}"/>
+    <hyperlink ref="I10" r:id="rId4" xr:uid="{2215A923-C24B-814E-98B7-6D7E33A957F4}"/>
+    <hyperlink ref="I11" r:id="rId5" xr:uid="{BA1FD78A-FC70-3448-9430-6AD2AAE5C113}"/>
+    <hyperlink ref="I14" r:id="rId6" xr:uid="{D46FA54C-F0C0-AD41-8AEC-7FDF7A69379C}"/>
+    <hyperlink ref="I17" r:id="rId7" xr:uid="{6F52A2EE-C700-244E-B27D-67B84397BB9A}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{E4A09A98-DB65-BC4B-AE2B-BEADAE2B6634}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>